<commit_message>
Upload linest ESP + upload data ESP
</commit_message>
<xml_diff>
--- a/LO6/ESP/data.xlsx
+++ b/LO6/ESP/data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erwinplanck/Desktop/Physics/Physics Lab III/LO6/ESP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35378B49-C455-D74A-9668-1CAC0A1680BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D336007B-B694-A14F-AE85-B91C06FA3CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15940" xr2:uid="{F39F0882-DD3A-9A44-8D56-DFB2621D2353}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -152,7 +153,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,6 +172,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -184,10 +191,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,14 +513,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32AE791A-ECD8-1A4E-B831-5010AD877A62}">
   <dimension ref="A2:U34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="16" max="16" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -604,12 +614,16 @@
         <f>1/(A5*0.000000001)^2</f>
         <v>2637492048373.5825</v>
       </c>
+      <c r="S5">
+        <f>1/A5^2</f>
+        <v>2.6374920483735823E-6</v>
+      </c>
       <c r="T5" cm="1">
         <f t="array" ref="T5:U9">LINEST(Q5:Q9,R5:R9,TRUE,TRUE)</f>
-        <v>1.0051629270950794E-14</v>
+        <v>9.9154161334764221E-15</v>
       </c>
       <c r="U5">
-        <v>1.5941200535883955</v>
+        <v>1.5947709472717151</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -629,11 +643,15 @@
         <f>1/(A7*0.000000001)^2</f>
         <v>2879566535393.9473</v>
       </c>
+      <c r="S6" t="e">
+        <f t="shared" ref="S6:S11" si="0">1/A6^2</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="T6">
-        <v>1.212384896104944E-15</v>
+        <v>8.6445723138521081E-16</v>
       </c>
       <c r="U6">
-        <v>4.0314818124465111E-3</v>
+        <v>2.874535650488405E-3</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
@@ -651,7 +669,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" ref="E6:E11" si="0">C7+D7/60</f>
+        <f t="shared" ref="E7:E11" si="1">C7+D7/60</f>
         <v>37.68333333333333</v>
       </c>
       <c r="F7" s="1"/>
@@ -662,37 +680,44 @@
         <v>20</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" ref="I6:I11" si="1">H7/60 +(360 - G7 + E7) + E7</f>
+        <f t="shared" ref="I7:I11" si="2">H7/60 +(360 - G7 + E7) + E7</f>
         <v>134.69999999999999</v>
       </c>
-      <c r="J7" s="1"/>
+      <c r="J7" s="1">
+        <f>(I7-INT(I7))*60</f>
+        <v>41.999999999999318</v>
+      </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1">
-        <f t="shared" ref="M6:M11" si="2">ABS((E7-I7)/2)</f>
+        <f t="shared" ref="M7:M11" si="3">ABS((E7-I7)/2)</f>
         <v>48.508333333333326</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1">
-        <f t="shared" ref="O6:O11" si="3">SIN(PI()*(M7+60)/360)/SIN(PI()*30/180)</f>
+        <f t="shared" ref="O7:Q11" si="4">SIN(PI()*(M7+60)/360)/SIN(PI()*30/180)</f>
         <v>1.6232329353072688</v>
       </c>
       <c r="P7">
-        <f t="shared" ref="P6:R11" si="4">1/(A7*0.000000001)^2</f>
+        <f t="shared" ref="P7:P11" si="5">1/(A7*0.000000001)^2</f>
         <v>2879566535393.9473</v>
       </c>
       <c r="Q7" s="2">
-        <v>1.6233179</v>
+        <v>1.6243367818618635</v>
       </c>
       <c r="R7">
         <f>1/(A9*0.000000001)^2</f>
         <v>3093589409115.2202</v>
       </c>
+      <c r="S7">
+        <f t="shared" si="0"/>
+        <v>2.879566535393948E-6</v>
+      </c>
       <c r="T7">
-        <v>0.95818069774326931</v>
+        <v>0.97770566521019298</v>
       </c>
       <c r="U7">
-        <v>1.4411247260621267E-3</v>
+        <v>1.0275537865696083E-3</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -705,6 +730,7 @@
       <c r="D8">
         <v>13</v>
       </c>
+      <c r="J8" s="4"/>
       <c r="Q8" s="2">
         <v>1.63328311</v>
       </c>
@@ -712,8 +738,12 @@
         <f>1/(A10*0.000000001)^2</f>
         <v>3770383636535.0166</v>
       </c>
+      <c r="S8" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="T8">
-        <v>68.73720837289099</v>
+        <v>131.56333316442354</v>
       </c>
       <c r="U8">
         <v>3</v>
@@ -721,20 +751,21 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9">
+        <f>AVERAGE(B9,568.3)</f>
         <v>568.54999999999995</v>
       </c>
       <c r="B9" s="1">
         <v>568.79999999999995</v>
       </c>
       <c r="C9" s="1">
-        <v>37.5</v>
+        <v>38</v>
       </c>
       <c r="D9" s="1">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
-        <v>37.9</v>
+        <f t="shared" si="1"/>
+        <v>38.1</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1">
@@ -744,23 +775,26 @@
         <v>8</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" si="1"/>
-        <v>134.93333333333334</v>
-      </c>
-      <c r="J9" s="1"/>
+        <f t="shared" si="2"/>
+        <v>135.33333333333334</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" ref="J8:J11" si="6">(I9-INT(I9))*60</f>
+        <v>20.000000000000568</v>
+      </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1">
-        <f t="shared" si="2"/>
-        <v>48.516666666666666</v>
+        <f t="shared" si="3"/>
+        <v>48.616666666666674</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1">
-        <f t="shared" si="3"/>
-        <v>1.6233178981000504</v>
+        <f t="shared" si="4"/>
+        <v>1.6243367818618635</v>
       </c>
       <c r="P9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3093589409115.2202</v>
       </c>
       <c r="Q9" s="2">
@@ -770,11 +804,15 @@
         <f>1/(A11*0.000000001)^2</f>
         <v>4031383473752.6343</v>
       </c>
+      <c r="S9">
+        <f t="shared" si="0"/>
+        <v>3.0935894091152201E-6</v>
+      </c>
       <c r="T9">
-        <v>1.4275621656071545E-4</v>
+        <v>1.3891335351925952E-4</v>
       </c>
       <c r="U9">
-        <v>6.2305214282029179E-6</v>
+        <v>3.1676003528806199E-6</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
@@ -791,7 +829,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38.533333333333331</v>
       </c>
       <c r="F10" s="1"/>
@@ -802,24 +840,31 @@
         <v>28</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>137.53333333333333</v>
       </c>
-      <c r="J10" s="1"/>
+      <c r="J10" s="1">
+        <f t="shared" si="6"/>
+        <v>31.999999999999886</v>
+      </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>49.5</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.633283110323358</v>
       </c>
       <c r="P10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3770383636535.0166</v>
+      </c>
+      <c r="S10">
+        <f>1/A10^2</f>
+        <v>3.7703836365350176E-6</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
@@ -837,7 +882,7 @@
         <v>22</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38.866666666666667</v>
       </c>
       <c r="F11" s="1"/>
@@ -848,24 +893,44 @@
         <v>19</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>138.05000000000001</v>
       </c>
-      <c r="J11" s="1"/>
+      <c r="J11" s="1">
+        <f t="shared" si="6"/>
+        <v>3.0000000000006821</v>
+      </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>49.591666666666669</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.6342059536669291</v>
       </c>
       <c r="P11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4031383473752.6343</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="0"/>
+        <v>4.0313834737526342E-6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="I13">
+        <f>11/60</f>
+        <v>0.18333333333333332</v>
+      </c>
+      <c r="J13">
+        <f>42/60</f>
+        <v>0.7</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
@@ -885,31 +950,31 @@
       </c>
       <c r="D16">
         <f>$D$15*0.001*2*$T$5/(A5^3 * 1E-27)</f>
-        <v>2585.0198622995135</v>
+        <v>2549.9893556636393</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D18">
-        <f t="shared" ref="D17:D23" si="5">$D$15*0.001*2*$T$5/(A7^3 * 1E-27)</f>
-        <v>2948.9528082470101</v>
+        <f t="shared" ref="D18:D22" si="7">$D$15*0.001*2*$T$5/(A7^3 * 1E-27)</f>
+        <v>2908.9905192043711</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D20">
-        <f t="shared" si="5"/>
-        <v>3283.7580792757612</v>
+        <f t="shared" si="7"/>
+        <v>3239.2587271182319</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D21">
-        <f t="shared" si="5"/>
-        <v>4418.3026240068066</v>
+        <f t="shared" si="7"/>
+        <v>4358.4286626315588</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D22">
-        <f t="shared" si="5"/>
-        <v>4884.9296386247252</v>
+        <f t="shared" si="7"/>
+        <v>4818.7322516656168</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
@@ -963,25 +1028,112 @@
       <c r="B30" t="s">
         <v>13</v>
       </c>
+      <c r="C30">
+        <f>289 + 26/60</f>
+        <v>289.43333333333334</v>
+      </c>
+      <c r="D30">
+        <v>333</v>
+      </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>14</v>
       </c>
+      <c r="C31">
+        <f>290 + 25/60</f>
+        <v>290.41666666666669</v>
+      </c>
+      <c r="D31">
+        <f>332 + 4/60</f>
+        <v>332.06666666666666</v>
+      </c>
+      <c r="E31">
+        <f>265.5 + 4/60</f>
+        <v>265.56666666666666</v>
+      </c>
+      <c r="F31">
+        <f>356 + 10/60</f>
+        <v>356.16666666666669</v>
+      </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <f>291 + 6/60</f>
+        <v>291.10000000000002</v>
+      </c>
+      <c r="D32">
+        <f>331 + 21/60</f>
+        <v>331.35</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <f>293 + 1/60</f>
+        <v>293.01666666666665</v>
+      </c>
+      <c r="D33">
+        <f>329 + 24/60</f>
+        <v>329.4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>17</v>
+      </c>
+      <c r="C34">
+        <f>293.5 + 12/60</f>
+        <v>293.7</v>
+      </c>
+      <c r="D34">
+        <f>328.5 + 11/60</f>
+        <v>328.68333333333334</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFF85A6-EC1A-6344-9316-72A27CE4A475}">
+  <dimension ref="B2:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>1.6215318773124865</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>1.6232329353072688</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>1.6243367818618635</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>1.633283110323358</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>1.6342059536669291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>